<commit_message>
added comments and README.md
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,6 +464,37 @@
         <v>45028.46605659319</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>5664786994</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>thecooldevv</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>The Dev</t>
+        </is>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>45028.49481748261</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>5845473123</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Prince</t>
+        </is>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>45029.39132129507</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>